<commit_message>
update csv files to correct a mistake
</commit_message>
<xml_diff>
--- a/data/topics_iphone_v2.xlsx
+++ b/data/topics_iphone_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90802B1-6916-4F61-8754-B64EBC68FFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9ACEEBB-83C7-480C-9107-66EBC6375D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="25580" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="topics_iphone_v2" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="545">
   <si>
     <t>year</t>
   </si>
@@ -1696,6 +1696,10 @@
   </si>
   <si>
     <t>In 2019, Apple faced a significant setback in China, with iPhone sales plummeting by 35%. This decline marked a stark contrast to the company's previous success and dominance in the tech industry. Local competitors like Huawei, with their culturally attuned and affordable products, were capturing the hearts and wallets of Chinese consumers, overshadowing the allure of the iPhone. Apple's struggle in China symbolized a pivotal moment, highlighting the challenges of maintaining market dominance amidst fierce local competition and changing consumer preferences. This period was a wake-up call for Apple, underscoring the need for strategic adaptation and resilience in the face of global market shifts.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AirPods, Bluetooth, Wireless Audio, Battery Life, Connectivity</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2036,8 +2040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C148" workbookViewId="0">
-      <selection activeCell="F171" sqref="F171"/>
+    <sheetView tabSelected="1" topLeftCell="C136" workbookViewId="0">
+      <selection activeCell="E147" sqref="E147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -4883,7 +4887,7 @@
         <v>58</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>471</v>
+        <v>544</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>471</v>

</xml_diff>